<commit_message>
Write To Excel Update
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arcadier\git\Trillia\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB878271-8276-4BF7-8E68-DABD85BBF80A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E36BF28-2DDF-42D6-BC04-BD8467F4368A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Category" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="Custom Fields" sheetId="6" r:id="rId6"/>
     <sheet name="AllCustomField" sheetId="7" r:id="rId7"/>
     <sheet name="Item List" sheetId="9" r:id="rId8"/>
+    <sheet name="Sample" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2581" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="1073">
   <si>
     <t>CategoryNametext</t>
   </si>
@@ -3250,13 +3251,20 @@
   </si>
   <si>
     <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item10.jpg</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>100.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3837,10 +3845,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="79.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4974,10 +4982,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="16.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" style="3" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="16.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="20.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -5841,15 +5849,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.7109375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="26" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="26" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" customWidth="true" style="26" width="46.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="26" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="26" width="38.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="26" width="46.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="26" width="14.140625" collapsed="true"/>
+    <col min="6" max="16384" style="26" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>844</v>
       </c>
@@ -6143,16 +6151,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7571,14 +7579,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="15" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -8678,11 +8686,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="64.5" x14ac:dyDescent="0.25">
@@ -11138,10 +11146,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -12162,21 +12170,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337AF865-08E8-4C8C-A074-848D6C202917}">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="76.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="76.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -15446,4 +15454,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E03EA7-0AF0-45C5-8798-242106C9C48B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>